<commit_message>
adapt data handling to isotope data
</commit_message>
<xml_diff>
--- a/mibipret/data/example_data.xlsx
+++ b/mibipret/data/example_data.xlsx
@@ -5,11 +5,13 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="contaminants" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="environment" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="metabolites" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="isotopes" sheetId="4" state="visible" r:id="rId5"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -21,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="45">
   <si>
     <t xml:space="preserve">sample_nr</t>
   </si>
@@ -119,7 +121,7 @@
     <t xml:space="preserve">methane</t>
   </si>
   <si>
-    <t xml:space="preserve">ironII</t>
+    <t xml:space="preserve">iron2</t>
   </si>
   <si>
     <t xml:space="preserve">manganese</t>
@@ -135,6 +137,27 @@
   </si>
   <si>
     <t xml:space="preserve">mg/L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">phenol</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cinnamic_acid</t>
+  </si>
+  <si>
+    <t xml:space="preserve">benzoic_acid</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ug/l</t>
+  </si>
+  <si>
+    <t xml:space="preserve">delta_13C-benzene</t>
+  </si>
+  <si>
+    <t xml:space="preserve">delta_2H-benzene</t>
+  </si>
+  <si>
+    <t xml:space="preserve">permil</t>
   </si>
 </sst>
 </file>
@@ -144,7 +167,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -172,6 +195,36 @@
       <sz val="11"/>
       <name val="Cambria"/>
       <family val="0"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="11"/>
+      <name val="Cambria"/>
+      <family val="1"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Cambria"/>
+      <family val="1"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="11"/>
+      <name val=""/>
+      <family val="0"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <charset val="1"/>
     </font>
   </fonts>
@@ -224,7 +277,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -234,6 +287,22 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -256,8 +325,8 @@
   </sheetPr>
   <dimension ref="A1:K6"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="1:1048576"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -490,11 +559,11 @@
   </sheetPr>
   <dimension ref="A1:P6"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="1:1048576"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1017" style="0" width="9.14"/>
   </cols>
@@ -797,6 +866,284 @@
       </c>
       <c r="P6" s="0" t="n">
         <v>0.1</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;Kffffff&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;KffffffPage &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:F6"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="1" style="0" width="8.54"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="5.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="10.4"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="9.63"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="E2" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="F2" s="0" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="2" t="n">
+        <v>-12</v>
+      </c>
+      <c r="D3" s="0" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="E3" s="0" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="F3" s="0" t="n">
+        <v>1.4</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" s="2" t="n">
+        <v>-15.5</v>
+      </c>
+      <c r="E4" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" s="2" t="n">
+        <v>-17</v>
+      </c>
+      <c r="D5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E5" s="0" t="n">
+        <v>11.4</v>
+      </c>
+      <c r="F5" s="0" t="n">
+        <v>5.4</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" s="2" t="n">
+        <v>-19</v>
+      </c>
+      <c r="D6" s="0" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="E6" s="0" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="F6" s="0" t="n">
+        <v>0.7</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;Kffffff&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;KffffffPage &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:E6"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D10" activeCellId="0" sqref="D10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="1" style="0" width="8.54"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="13.48"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="12.71"/>
+  </cols>
+  <sheetData>
+    <row r="1" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="E2" s="0" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="2" t="n">
+        <v>-12</v>
+      </c>
+      <c r="D3" s="0" t="n">
+        <v>-26.1</v>
+      </c>
+      <c r="E3" s="0" t="n">
+        <v>-106</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" s="2" t="n">
+        <v>-15.5</v>
+      </c>
+      <c r="D4" s="0" t="n">
+        <v>-25.8</v>
+      </c>
+      <c r="E4" s="0" t="n">
+        <v>-110</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" s="2" t="n">
+        <v>-17</v>
+      </c>
+      <c r="D5" s="0" t="n">
+        <v>-24.1</v>
+      </c>
+      <c r="E5" s="0" t="n">
+        <v>-118</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" s="2" t="n">
+        <v>-19</v>
+      </c>
+      <c r="D6" s="0" t="n">
+        <v>-24.1</v>
+      </c>
+      <c r="E6" s="0" t="n">
+        <v>-117</v>
       </c>
     </row>
   </sheetData>

</xml_diff>